<commit_message>
Pre-process data and thereafter run specified model
</commit_message>
<xml_diff>
--- a/results/randomForests.xlsx
+++ b/results/randomForests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">bestHyperparameters</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">testAccuracy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{'n_estimators': 1000, 'min_samples_split': 2, 'min_samples_leaf': 2, 'max_features': 'sqrt', 'max_depth': 4, 'criterion': 'entropy', 'bootstrap': False}</t>
   </si>
 </sst>
 </file>
@@ -146,10 +143,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -172,17 +169,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>0.717</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>